<commit_message>
regression R2 tables and transtion by type tables
</commit_message>
<xml_diff>
--- a/my_code/model_uncert/input/50_50/MH_trans.xlsx
+++ b/my_code/model_uncert/input/50_50/MH_trans.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="7">
   <si>
     <t>Bad MH Type : % transition from bad mental health</t>
   </si>
@@ -137,37 +137,37 @@
         <v>25</v>
       </c>
       <c r="B3">
-        <v>0.788637513571256</v>
+        <v>0.79295224824335975</v>
       </c>
       <c r="C3">
-        <v>0.21136248642874406</v>
+        <v>0.20704775175664014</v>
       </c>
       <c r="H3">
         <v>25</v>
       </c>
       <c r="I3">
-        <v>0.22171544056234477</v>
+        <v>0.39846924608182327</v>
       </c>
       <c r="J3">
-        <v>0.77828455943765518</v>
+        <v>0.60153075391817667</v>
       </c>
       <c r="N3">
         <v>25</v>
       </c>
       <c r="O3">
-        <v>0.47236731906017326</v>
+        <v>0.34147074017128831</v>
       </c>
       <c r="P3">
-        <v>0.52763268093982674</v>
+        <v>0.65852925982871169</v>
       </c>
       <c r="T3">
         <v>25</v>
       </c>
       <c r="U3">
-        <v>0.8634349771870915</v>
+        <v>0.81176563753524345</v>
       </c>
       <c r="V3">
-        <v>0.13656502281290855</v>
+        <v>0.18823436246475661</v>
       </c>
     </row>
     <row r="4">
@@ -175,37 +175,37 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>0.7742447505071679</v>
+        <v>0.81004013056206992</v>
       </c>
       <c r="C4">
-        <v>0.2257552494928321</v>
+        <v>0.18995986943793006</v>
       </c>
       <c r="H4">
         <v>26</v>
       </c>
       <c r="I4">
-        <v>0.25617381231136582</v>
+        <v>0.327600759091908</v>
       </c>
       <c r="J4">
-        <v>0.74382618768863429</v>
+        <v>0.67239924090809189</v>
       </c>
       <c r="N4">
         <v>26</v>
       </c>
       <c r="O4">
-        <v>0.45781814418212063</v>
+        <v>0.33108818094901715</v>
       </c>
       <c r="P4">
-        <v>0.54218185581787948</v>
+        <v>0.66891181905098296</v>
       </c>
       <c r="T4">
         <v>26</v>
       </c>
       <c r="U4">
-        <v>0.85429714762456188</v>
+        <v>0.79553759989320449</v>
       </c>
       <c r="V4">
-        <v>0.14570285237543809</v>
+        <v>0.20446240010679562</v>
       </c>
     </row>
     <row r="5">
@@ -213,37 +213,37 @@
         <v>27</v>
       </c>
       <c r="B5">
-        <v>0.73844402248006036</v>
+        <v>0.7437675836296167</v>
       </c>
       <c r="C5">
-        <v>0.26155597751993975</v>
+        <v>0.2562324163703833</v>
       </c>
       <c r="H5">
         <v>27</v>
       </c>
       <c r="I5">
-        <v>0.14905896660834567</v>
+        <v>0.1655864864647453</v>
       </c>
       <c r="J5">
-        <v>0.85094103339165439</v>
+        <v>0.83441351353525473</v>
       </c>
       <c r="N5">
         <v>27</v>
       </c>
       <c r="O5">
-        <v>0.45337333424219878</v>
+        <v>0.377288977206929</v>
       </c>
       <c r="P5">
-        <v>0.54662666575780128</v>
+        <v>0.622711022793071</v>
       </c>
       <c r="T5">
         <v>27</v>
       </c>
       <c r="U5">
-        <v>0.88004220790989918</v>
+        <v>0.79151316024510365</v>
       </c>
       <c r="V5">
-        <v>0.11995779209010077</v>
+        <v>0.20848683975489632</v>
       </c>
     </row>
     <row r="6">
@@ -251,37 +251,37 @@
         <v>28</v>
       </c>
       <c r="B6">
-        <v>0.77171694206595132</v>
+        <v>0.8166082179138644</v>
       </c>
       <c r="C6">
-        <v>0.22828305793404863</v>
+        <v>0.18339178208613566</v>
       </c>
       <c r="H6">
         <v>28</v>
       </c>
       <c r="I6">
-        <v>0.21174231494586393</v>
+        <v>0.38379142304010894</v>
       </c>
       <c r="J6">
-        <v>0.78825768505413607</v>
+        <v>0.61620857695989106</v>
       </c>
       <c r="N6">
         <v>28</v>
       </c>
       <c r="O6">
-        <v>0.39303463626504803</v>
+        <v>0.23193326816446602</v>
       </c>
       <c r="P6">
-        <v>0.60696536373495202</v>
+        <v>0.76806673183553398</v>
       </c>
       <c r="T6">
         <v>28</v>
       </c>
       <c r="U6">
-        <v>0.87069013894626235</v>
+        <v>0.77202830035980952</v>
       </c>
       <c r="V6">
-        <v>0.12930986105373762</v>
+        <v>0.22797169964019051</v>
       </c>
     </row>
     <row r="7">
@@ -289,37 +289,37 @@
         <v>29</v>
       </c>
       <c r="B7">
-        <v>0.75830367252985897</v>
+        <v>0.79599521172206422</v>
       </c>
       <c r="C7">
-        <v>0.24169632747014097</v>
+        <v>0.20400478827793578</v>
       </c>
       <c r="H7">
         <v>29</v>
       </c>
       <c r="I7">
-        <v>0.12963330825637748</v>
+        <v>0.37505296861108012</v>
       </c>
       <c r="J7">
-        <v>0.87036669174362247</v>
+        <v>0.62494703138891983</v>
       </c>
       <c r="N7">
         <v>29</v>
       </c>
       <c r="O7">
-        <v>0.47800358401242965</v>
+        <v>0.32272766733835184</v>
       </c>
       <c r="P7">
-        <v>0.52199641598757029</v>
+        <v>0.6772723326616481</v>
       </c>
       <c r="T7">
         <v>29</v>
       </c>
       <c r="U7">
-        <v>0.85991702285917049</v>
+        <v>0.73943720303714389</v>
       </c>
       <c r="V7">
-        <v>0.14008297714082951</v>
+        <v>0.260562796962856</v>
       </c>
     </row>
     <row r="8">
@@ -327,37 +327,37 @@
         <v>30</v>
       </c>
       <c r="B8">
-        <v>0.77213054228067457</v>
+        <v>0.78060319075451656</v>
       </c>
       <c r="C8">
-        <v>0.22786945771932557</v>
+        <v>0.21939680924548349</v>
       </c>
       <c r="H8">
         <v>30</v>
       </c>
       <c r="I8">
-        <v>0.20247714883755955</v>
+        <v>0.43247388190257191</v>
       </c>
       <c r="J8">
-        <v>0.79752285116244048</v>
+        <v>0.56752611809742814</v>
       </c>
       <c r="N8">
         <v>30</v>
       </c>
       <c r="O8">
-        <v>0.44523523203688936</v>
+        <v>0.43299490687520598</v>
       </c>
       <c r="P8">
-        <v>0.55476476796311047</v>
+        <v>0.56700509312479397</v>
       </c>
       <c r="T8">
         <v>30</v>
       </c>
       <c r="U8">
-        <v>0.86592427184998966</v>
+        <v>0.82321988920974487</v>
       </c>
       <c r="V8">
-        <v>0.13407572815001031</v>
+        <v>0.17678011079025518</v>
       </c>
     </row>
     <row r="9">
@@ -365,37 +365,37 @@
         <v>31</v>
       </c>
       <c r="B9">
-        <v>0.74822320689433264</v>
+        <v>0.76329477373856303</v>
       </c>
       <c r="C9">
-        <v>0.25177679310566753</v>
+        <v>0.23670522626143697</v>
       </c>
       <c r="H9">
         <v>31</v>
       </c>
       <c r="I9">
-        <v>0.21562120621710607</v>
+        <v>0.35356897314111074</v>
       </c>
       <c r="J9">
-        <v>0.78437879378289399</v>
+        <v>0.64643102685888909</v>
       </c>
       <c r="N9">
         <v>31</v>
       </c>
       <c r="O9">
-        <v>0.42178895991435428</v>
+        <v>0.24099460431003675</v>
       </c>
       <c r="P9">
-        <v>0.57821104008564572</v>
+        <v>0.75900539568996328</v>
       </c>
       <c r="T9">
         <v>31</v>
       </c>
       <c r="U9">
-        <v>0.87191041484691634</v>
+        <v>0.80353847964051472</v>
       </c>
       <c r="V9">
-        <v>0.12808958515308375</v>
+        <v>0.19646152035948525</v>
       </c>
     </row>
     <row r="10">
@@ -403,37 +403,37 @@
         <v>32</v>
       </c>
       <c r="B10">
-        <v>0.78255426732497579</v>
+        <v>0.80189472061670497</v>
       </c>
       <c r="C10">
-        <v>0.21744573267502407</v>
+        <v>0.19810527938329497</v>
       </c>
       <c r="H10">
         <v>32</v>
       </c>
       <c r="I10">
-        <v>0.28664544393512803</v>
+        <v>0.44060605099208949</v>
       </c>
       <c r="J10">
-        <v>0.71335455606487208</v>
+        <v>0.55939394900791062</v>
       </c>
       <c r="N10">
         <v>32</v>
       </c>
       <c r="O10">
-        <v>0.44818861652822117</v>
+        <v>0.32840862822797379</v>
       </c>
       <c r="P10">
-        <v>0.55181138347177894</v>
+        <v>0.67159137177202632</v>
       </c>
       <c r="T10">
         <v>32</v>
       </c>
       <c r="U10">
-        <v>0.85289662311980508</v>
+        <v>0.80231062707507883</v>
       </c>
       <c r="V10">
-        <v>0.14710337688019492</v>
+        <v>0.19768937292492111</v>
       </c>
     </row>
     <row r="11">
@@ -441,37 +441,37 @@
         <v>33</v>
       </c>
       <c r="B11">
-        <v>0.74794153228292604</v>
+        <v>0.77418609074781686</v>
       </c>
       <c r="C11">
-        <v>0.25205846771707391</v>
+        <v>0.22581390925218314</v>
       </c>
       <c r="H11">
         <v>33</v>
       </c>
       <c r="I11">
-        <v>0.11352127751059682</v>
+        <v>0.29675507153464709</v>
       </c>
       <c r="J11">
-        <v>0.88647872248940318</v>
+        <v>0.70324492846535291</v>
       </c>
       <c r="N11">
         <v>33</v>
       </c>
       <c r="O11">
-        <v>0.43220570545520337</v>
+        <v>0.24061969479235051</v>
       </c>
       <c r="P11">
-        <v>0.56779429454479657</v>
+        <v>0.75938030520764943</v>
       </c>
       <c r="T11">
         <v>33</v>
       </c>
       <c r="U11">
-        <v>0.88303712101872001</v>
+        <v>0.79090791087787216</v>
       </c>
       <c r="V11">
-        <v>0.11696287898128001</v>
+        <v>0.20909208912212793</v>
       </c>
     </row>
     <row r="12">
@@ -479,37 +479,37 @@
         <v>34</v>
       </c>
       <c r="B12">
-        <v>0.7653745484436888</v>
+        <v>0.8156755586451383</v>
       </c>
       <c r="C12">
-        <v>0.2346254515563112</v>
+        <v>0.18432444135486176</v>
       </c>
       <c r="H12">
         <v>34</v>
       </c>
       <c r="I12">
-        <v>0.25265701970161036</v>
+        <v>0.34491917450721499</v>
       </c>
       <c r="J12">
-        <v>0.74734298029838975</v>
+        <v>0.65508082549278501</v>
       </c>
       <c r="N12">
         <v>34</v>
       </c>
       <c r="O12">
-        <v>0.46065764172367374</v>
+        <v>0.22945203461989308</v>
       </c>
       <c r="P12">
-        <v>0.53934235827632626</v>
+        <v>0.77054796538010706</v>
       </c>
       <c r="T12">
         <v>34</v>
       </c>
       <c r="U12">
-        <v>0.87037264020630867</v>
+        <v>0.79043508711619481</v>
       </c>
       <c r="V12">
-        <v>0.12962735979369122</v>
+        <v>0.20956491288380522</v>
       </c>
     </row>
     <row r="13">
@@ -517,37 +517,37 @@
         <v>35</v>
       </c>
       <c r="B13">
-        <v>0.76193450942550101</v>
+        <v>0.82853435903839812</v>
       </c>
       <c r="C13">
-        <v>0.23806549057449902</v>
+        <v>0.17146564096160191</v>
       </c>
       <c r="H13">
         <v>35</v>
       </c>
       <c r="I13">
-        <v>0.28518952043760287</v>
+        <v>0.38174144317001441</v>
       </c>
       <c r="J13">
-        <v>0.71481047956239707</v>
+        <v>0.61825855682998554</v>
       </c>
       <c r="N13">
         <v>35</v>
       </c>
       <c r="O13">
-        <v>0.48257652030509912</v>
+        <v>0.22164468396282969</v>
       </c>
       <c r="P13">
-        <v>0.51742347969490088</v>
+        <v>0.77835531603717034</v>
       </c>
       <c r="T13">
         <v>35</v>
       </c>
       <c r="U13">
-        <v>0.86711046378449164</v>
+        <v>0.79206224986257112</v>
       </c>
       <c r="V13">
-        <v>0.13288953621550834</v>
+        <v>0.20793775013742893</v>
       </c>
     </row>
     <row r="14">
@@ -555,37 +555,37 @@
         <v>36</v>
       </c>
       <c r="B14">
-        <v>0.7787049283200328</v>
+        <v>0.83816747273284453</v>
       </c>
       <c r="C14">
-        <v>0.22129507167996718</v>
+        <v>0.16183252726715541</v>
       </c>
       <c r="H14">
         <v>36</v>
       </c>
       <c r="I14">
-        <v>0.23407889170785628</v>
+        <v>0.36088062025980905</v>
       </c>
       <c r="J14">
-        <v>0.76592110829214377</v>
+        <v>0.63911937974019095</v>
       </c>
       <c r="N14">
         <v>36</v>
       </c>
       <c r="O14">
-        <v>0.42358544765102668</v>
+        <v>0.27646691930229927</v>
       </c>
       <c r="P14">
-        <v>0.57641455234897343</v>
+        <v>0.72353308069770084</v>
       </c>
       <c r="T14">
         <v>36</v>
       </c>
       <c r="U14">
-        <v>0.89457161249068295</v>
+        <v>0.80676094929616737</v>
       </c>
       <c r="V14">
-        <v>0.10542838750931703</v>
+        <v>0.19323905070383268</v>
       </c>
     </row>
     <row r="15">
@@ -593,37 +593,37 @@
         <v>37</v>
       </c>
       <c r="B15">
-        <v>0.77745040624472972</v>
+        <v>0.83786288469470604</v>
       </c>
       <c r="C15">
-        <v>0.22254959375527031</v>
+        <v>0.16213711530529398</v>
       </c>
       <c r="H15">
         <v>37</v>
       </c>
       <c r="I15">
-        <v>0.14765834045891046</v>
+        <v>0.37779673859250135</v>
       </c>
       <c r="J15">
-        <v>0.85234165954108942</v>
+        <v>0.6222032614074986</v>
       </c>
       <c r="N15">
         <v>37</v>
       </c>
       <c r="O15">
-        <v>0.43712713729454206</v>
+        <v>0.27469538973018603</v>
       </c>
       <c r="P15">
-        <v>0.56287286270545789</v>
+        <v>0.72530461026981397</v>
       </c>
       <c r="T15">
         <v>37</v>
       </c>
       <c r="U15">
-        <v>0.87109153741540801</v>
+        <v>0.77243641875385993</v>
       </c>
       <c r="V15">
-        <v>0.12890846258459193</v>
+        <v>0.22756358124614007</v>
       </c>
     </row>
     <row r="16">
@@ -631,37 +631,37 @@
         <v>38</v>
       </c>
       <c r="B16">
-        <v>0.76439208599852104</v>
+        <v>0.81844704294646187</v>
       </c>
       <c r="C16">
-        <v>0.23560791400147887</v>
+        <v>0.18155295705353827</v>
       </c>
       <c r="H16">
         <v>38</v>
       </c>
       <c r="I16">
-        <v>0.15415569183766289</v>
+        <v>0.3996007936646811</v>
       </c>
       <c r="J16">
-        <v>0.84584430816233702</v>
+        <v>0.60039920633531885</v>
       </c>
       <c r="N16">
         <v>38</v>
       </c>
       <c r="O16">
-        <v>0.43454599810658534</v>
+        <v>0.33815716379030175</v>
       </c>
       <c r="P16">
-        <v>0.56545400189341455</v>
+        <v>0.6618428362096983</v>
       </c>
       <c r="T16">
         <v>38</v>
       </c>
       <c r="U16">
-        <v>0.88520602660316783</v>
+        <v>0.81592151802059498</v>
       </c>
       <c r="V16">
-        <v>0.11479397339683209</v>
+        <v>0.1840784819794051</v>
       </c>
     </row>
     <row r="17">
@@ -669,37 +669,37 @@
         <v>39</v>
       </c>
       <c r="B17">
-        <v>0.76286611108385149</v>
+        <v>0.84874835372470347</v>
       </c>
       <c r="C17">
-        <v>0.23713388891614851</v>
+        <v>0.15125164627529644</v>
       </c>
       <c r="H17">
         <v>39</v>
       </c>
       <c r="I17">
-        <v>0.16787843886393117</v>
+        <v>0.37016038997702061</v>
       </c>
       <c r="J17">
-        <v>0.83212156113606883</v>
+        <v>0.62983961002297939</v>
       </c>
       <c r="N17">
         <v>39</v>
       </c>
       <c r="O17">
-        <v>0.45853939619052525</v>
+        <v>0.54742158896389359</v>
       </c>
       <c r="P17">
-        <v>0.54146060380947469</v>
+        <v>0.45257841103610635</v>
       </c>
       <c r="T17">
         <v>39</v>
       </c>
       <c r="U17">
-        <v>0.89644368855863044</v>
+        <v>0.80504052383312741</v>
       </c>
       <c r="V17">
-        <v>0.10355631144136954</v>
+        <v>0.19495947616687268</v>
       </c>
     </row>
     <row r="18">
@@ -707,37 +707,37 @@
         <v>40</v>
       </c>
       <c r="B18">
-        <v>0.76277805755244921</v>
+        <v>0.80896762294241997</v>
       </c>
       <c r="C18">
-        <v>0.23722194244755079</v>
+        <v>0.19103237705758008</v>
       </c>
       <c r="H18">
         <v>40</v>
       </c>
       <c r="I18">
-        <v>0.25604760142835492</v>
+        <v>0.34591297287743422</v>
       </c>
       <c r="J18">
-        <v>0.74395239857164508</v>
+        <v>0.65408702712256572</v>
       </c>
       <c r="N18">
         <v>40</v>
       </c>
       <c r="O18">
-        <v>0.49680966400651577</v>
+        <v>0.30307795448711511</v>
       </c>
       <c r="P18">
-        <v>0.50319033599348428</v>
+        <v>0.69692204551288495</v>
       </c>
       <c r="T18">
         <v>40</v>
       </c>
       <c r="U18">
-        <v>0.90523476748299159</v>
+        <v>0.82876466217770939</v>
       </c>
       <c r="V18">
-        <v>0.094765232517008455</v>
+        <v>0.17123533782229064</v>
       </c>
     </row>
     <row r="19">
@@ -745,37 +745,37 @@
         <v>41</v>
       </c>
       <c r="B19">
-        <v>0.76197269205237261</v>
+        <v>0.82812496873571539</v>
       </c>
       <c r="C19">
-        <v>0.23802730794762733</v>
+        <v>0.17187503126428455</v>
       </c>
       <c r="H19">
         <v>41</v>
       </c>
       <c r="I19">
-        <v>0.22714089749447849</v>
+        <v>0.45784836871937473</v>
       </c>
       <c r="J19">
-        <v>0.77285910250552148</v>
+        <v>0.54215163128062527</v>
       </c>
       <c r="N19">
         <v>41</v>
       </c>
       <c r="O19">
-        <v>0.48906749065107896</v>
+        <v>0.29083945587489496</v>
       </c>
       <c r="P19">
-        <v>0.51093250934892109</v>
+        <v>0.70916054412510499</v>
       </c>
       <c r="T19">
         <v>41</v>
       </c>
       <c r="U19">
-        <v>0.90000885124943875</v>
+        <v>0.83387521866248671</v>
       </c>
       <c r="V19">
-        <v>0.099991148750561337</v>
+        <v>0.16612478133751332</v>
       </c>
     </row>
     <row r="20">
@@ -783,37 +783,37 @@
         <v>42</v>
       </c>
       <c r="B20">
-        <v>0.76402333526356825</v>
+        <v>0.82502113135454302</v>
       </c>
       <c r="C20">
-        <v>0.23597666473643172</v>
+        <v>0.174978868645457</v>
       </c>
       <c r="H20">
         <v>42</v>
       </c>
       <c r="I20">
-        <v>0.13232239144530372</v>
+        <v>0.3354301405179328</v>
       </c>
       <c r="J20">
-        <v>0.86767760855469622</v>
+        <v>0.66456985948206726</v>
       </c>
       <c r="N20">
         <v>42</v>
       </c>
       <c r="O20">
-        <v>0.47246104590095239</v>
+        <v>0.29886375689697076</v>
       </c>
       <c r="P20">
-        <v>0.52753895409904761</v>
+        <v>0.70113624310302913</v>
       </c>
       <c r="T20">
         <v>42</v>
       </c>
       <c r="U20">
-        <v>0.89633327357903858</v>
+        <v>0.83981992698498176</v>
       </c>
       <c r="V20">
-        <v>0.10366672642096138</v>
+        <v>0.16018007301501819</v>
       </c>
     </row>
     <row r="21">
@@ -821,37 +821,37 @@
         <v>43</v>
       </c>
       <c r="B21">
-        <v>0.73590273165777143</v>
+        <v>0.82827367718307232</v>
       </c>
       <c r="C21">
-        <v>0.26409726834222852</v>
+        <v>0.17172632281692765</v>
       </c>
       <c r="H21">
         <v>43</v>
       </c>
       <c r="I21">
-        <v>0.17131255545973734</v>
+        <v>0.31566100170672645</v>
       </c>
       <c r="J21">
-        <v>0.82868744454026277</v>
+        <v>0.68433899829327349</v>
       </c>
       <c r="N21">
         <v>43</v>
       </c>
       <c r="O21">
-        <v>0.42576093105932183</v>
+        <v>0.23806914902808451</v>
       </c>
       <c r="P21">
-        <v>0.57423906894067822</v>
+        <v>0.76193085097191549</v>
       </c>
       <c r="T21">
         <v>43</v>
       </c>
       <c r="U21">
-        <v>0.91050101053020771</v>
+        <v>0.83665249367177241</v>
       </c>
       <c r="V21">
-        <v>0.089498989469792248</v>
+        <v>0.1633475063282277</v>
       </c>
     </row>
     <row r="22">
@@ -859,37 +859,37 @@
         <v>44</v>
       </c>
       <c r="B22">
-        <v>0.73347486632835202</v>
+        <v>0.80168579718869171</v>
       </c>
       <c r="C22">
-        <v>0.26652513367164804</v>
+        <v>0.19831420281130829</v>
       </c>
       <c r="H22">
         <v>44</v>
       </c>
       <c r="I22">
-        <v>0.24363070458576028</v>
+        <v>0.33675202402353022</v>
       </c>
       <c r="J22">
-        <v>0.75636929541423958</v>
+        <v>0.66324797597646978</v>
       </c>
       <c r="N22">
         <v>44</v>
       </c>
       <c r="O22">
-        <v>0.46801388752374851</v>
+        <v>0.37561623461648797</v>
       </c>
       <c r="P22">
-        <v>0.53198611247625149</v>
+        <v>0.62438376538351215</v>
       </c>
       <c r="T22">
         <v>44</v>
       </c>
       <c r="U22">
-        <v>0.89913807725932715</v>
+        <v>0.82423463327258417</v>
       </c>
       <c r="V22">
-        <v>0.10086192274067278</v>
+        <v>0.1757653667274158</v>
       </c>
     </row>
     <row r="23">
@@ -897,37 +897,37 @@
         <v>45</v>
       </c>
       <c r="B23">
-        <v>0.7584248388895044</v>
+        <v>0.80465899925630169</v>
       </c>
       <c r="C23">
-        <v>0.24157516111049562</v>
+        <v>0.19534100074369834</v>
       </c>
       <c r="H23">
         <v>45</v>
       </c>
       <c r="I23">
-        <v>0.22567139213458526</v>
+        <v>0.35467814763986494</v>
       </c>
       <c r="J23">
-        <v>0.7743286078654148</v>
+        <v>0.64532185236013506</v>
       </c>
       <c r="N23">
         <v>45</v>
       </c>
       <c r="O23">
-        <v>0.4643863634233763</v>
+        <v>0.26571767684165587</v>
       </c>
       <c r="P23">
-        <v>0.53561363657662375</v>
+        <v>0.73428232315834407</v>
       </c>
       <c r="T23">
         <v>45</v>
       </c>
       <c r="U23">
-        <v>0.88714473317393727</v>
+        <v>0.81875973297749816</v>
       </c>
       <c r="V23">
-        <v>0.11285526682606267</v>
+        <v>0.18124026702250193</v>
       </c>
     </row>
     <row r="24">
@@ -935,37 +935,37 @@
         <v>46</v>
       </c>
       <c r="B24">
-        <v>0.76439331230838525</v>
+        <v>0.8180915090089288</v>
       </c>
       <c r="C24">
-        <v>0.23560668769161469</v>
+        <v>0.18190849099107115</v>
       </c>
       <c r="H24">
         <v>46</v>
       </c>
       <c r="I24">
-        <v>0.26793774749566834</v>
+        <v>0.42297318366224712</v>
       </c>
       <c r="J24">
-        <v>0.73206225250433166</v>
+        <v>0.57702681633775288</v>
       </c>
       <c r="N24">
         <v>46</v>
       </c>
       <c r="O24">
-        <v>0.48982901110559585</v>
+        <v>0.37312107968661301</v>
       </c>
       <c r="P24">
-        <v>0.51017098889440415</v>
+        <v>0.62687892031338699</v>
       </c>
       <c r="T24">
         <v>46</v>
       </c>
       <c r="U24">
-        <v>0.87783350005795857</v>
+        <v>0.81018243411357804</v>
       </c>
       <c r="V24">
-        <v>0.12216649994204137</v>
+        <v>0.18981756588642185</v>
       </c>
     </row>
     <row r="25">
@@ -973,37 +973,37 @@
         <v>47</v>
       </c>
       <c r="B25">
-        <v>0.71206826234659926</v>
+        <v>0.7427825010066168</v>
       </c>
       <c r="C25">
-        <v>0.28793173765340085</v>
+        <v>0.25721749899338314</v>
       </c>
       <c r="H25">
         <v>47</v>
       </c>
       <c r="I25">
-        <v>0.19606691125162051</v>
+        <v>0.37420833154916228</v>
       </c>
       <c r="J25">
-        <v>0.80393308874837954</v>
+        <v>0.62579166845083778</v>
       </c>
       <c r="N25">
         <v>47</v>
       </c>
       <c r="O25">
-        <v>0.45736624582130003</v>
+        <v>0.26818879298068821</v>
       </c>
       <c r="P25">
-        <v>0.54263375417869997</v>
+        <v>0.73181120701931179</v>
       </c>
       <c r="T25">
         <v>47</v>
       </c>
       <c r="U25">
-        <v>0.88551871723047249</v>
+        <v>0.82388406935660907</v>
       </c>
       <c r="V25">
-        <v>0.11448128276952742</v>
+        <v>0.1761159306433909</v>
       </c>
     </row>
     <row r="26">
@@ -1011,37 +1011,37 @@
         <v>48</v>
       </c>
       <c r="B26">
-        <v>0.75065556558101021</v>
+        <v>0.85499105161373601</v>
       </c>
       <c r="C26">
-        <v>0.24934443441898974</v>
+        <v>0.14500894838626402</v>
       </c>
       <c r="H26">
         <v>48</v>
       </c>
       <c r="I26">
-        <v>0.20058161152826098</v>
+        <v>0.36239906726373733</v>
       </c>
       <c r="J26">
-        <v>0.79941838847173896</v>
+        <v>0.63760093273626262</v>
       </c>
       <c r="N26">
         <v>48</v>
       </c>
       <c r="O26">
-        <v>0.46108669589982237</v>
+        <v>0.35183526165558332</v>
       </c>
       <c r="P26">
-        <v>0.53891330410017768</v>
+        <v>0.64816473834441668</v>
       </c>
       <c r="T26">
         <v>48</v>
       </c>
       <c r="U26">
-        <v>0.88433369028096831</v>
+        <v>0.82620496428620693</v>
       </c>
       <c r="V26">
-        <v>0.11566630971903175</v>
+        <v>0.17379503571379301</v>
       </c>
     </row>
     <row r="27">
@@ -1049,37 +1049,37 @@
         <v>49</v>
       </c>
       <c r="B27">
-        <v>0.74877945718277028</v>
+        <v>0.82152249715190895</v>
       </c>
       <c r="C27">
-        <v>0.25122054281722966</v>
+        <v>0.17847750284809114</v>
       </c>
       <c r="H27">
         <v>49</v>
       </c>
       <c r="I27">
-        <v>0.17771192043035916</v>
+        <v>0.35778602698956324</v>
       </c>
       <c r="J27">
-        <v>0.82228807956964078</v>
+        <v>0.6422139730104367</v>
       </c>
       <c r="N27">
         <v>49</v>
       </c>
       <c r="O27">
-        <v>0.48711793427060279</v>
+        <v>0.51329310637769854</v>
       </c>
       <c r="P27">
-        <v>0.5128820657293971</v>
+        <v>0.48670689362230152</v>
       </c>
       <c r="T27">
         <v>49</v>
       </c>
       <c r="U27">
-        <v>0.88921778132602747</v>
+        <v>0.81047100970417119</v>
       </c>
       <c r="V27">
-        <v>0.11078221867397263</v>
+        <v>0.18952899029582884</v>
       </c>
     </row>
     <row r="28">
@@ -1087,37 +1087,37 @@
         <v>50</v>
       </c>
       <c r="B28">
-        <v>0.76733348599800311</v>
+        <v>0.78685710948105059</v>
       </c>
       <c r="C28">
-        <v>0.23266651400199681</v>
+        <v>0.21314289051894938</v>
       </c>
       <c r="H28">
         <v>50</v>
       </c>
       <c r="I28">
-        <v>0.20282882651898076</v>
+        <v>0.41294149791167611</v>
       </c>
       <c r="J28">
-        <v>0.79717117348101929</v>
+        <v>0.587058502088324</v>
       </c>
       <c r="N28">
         <v>50</v>
       </c>
       <c r="O28">
-        <v>0.42820034559846593</v>
+        <v>0.36374088280371714</v>
       </c>
       <c r="P28">
-        <v>0.57179965440153391</v>
+        <v>0.63625911719628292</v>
       </c>
       <c r="T28">
         <v>50</v>
       </c>
       <c r="U28">
-        <v>0.89042298668436026</v>
+        <v>0.84654378212859616</v>
       </c>
       <c r="V28">
-        <v>0.10957701331563977</v>
+        <v>0.15345621787140379</v>
       </c>
     </row>
     <row r="29">
@@ -1125,37 +1125,37 @@
         <v>51</v>
       </c>
       <c r="B29">
-        <v>0.77030568513489117</v>
+        <v>0.81723867716620902</v>
       </c>
       <c r="C29">
-        <v>0.22969431486510872</v>
+        <v>0.18276132283379093</v>
       </c>
       <c r="H29">
         <v>51</v>
       </c>
       <c r="I29">
-        <v>0.23907292502870489</v>
+        <v>0.39415759539392142</v>
       </c>
       <c r="J29">
-        <v>0.76092707497129508</v>
+        <v>0.60584240460607863</v>
       </c>
       <c r="N29">
         <v>51</v>
       </c>
       <c r="O29">
-        <v>0.49173204291069866</v>
+        <v>0.37451251214701281</v>
       </c>
       <c r="P29">
-        <v>0.50826795708930128</v>
+        <v>0.62548748785298713</v>
       </c>
       <c r="T29">
         <v>51</v>
       </c>
       <c r="U29">
-        <v>0.89851350108190298</v>
+        <v>0.84487292911616474</v>
       </c>
       <c r="V29">
-        <v>0.10148649891809713</v>
+        <v>0.15512707088383521</v>
       </c>
     </row>
     <row r="30">
@@ -1163,37 +1163,37 @@
         <v>52</v>
       </c>
       <c r="B30">
-        <v>0.73593689351671931</v>
+        <v>0.78421578382239543</v>
       </c>
       <c r="C30">
-        <v>0.2640631064832808</v>
+        <v>0.21578421617760457</v>
       </c>
       <c r="H30">
         <v>52</v>
       </c>
       <c r="I30">
-        <v>0.22103010517276059</v>
+        <v>0.34003428832993376</v>
       </c>
       <c r="J30">
-        <v>0.77896989482723933</v>
+        <v>0.65996571167006624</v>
       </c>
       <c r="N30">
         <v>52</v>
       </c>
       <c r="O30">
-        <v>0.45925574791329837</v>
+        <v>0.40305116192114832</v>
       </c>
       <c r="P30">
-        <v>0.54074425208670174</v>
+        <v>0.59694883807885168</v>
       </c>
       <c r="T30">
         <v>52</v>
       </c>
       <c r="U30">
-        <v>0.8920865121220598</v>
+        <v>0.83014188789191545</v>
       </c>
       <c r="V30">
-        <v>0.1079134878779401</v>
+        <v>0.16985811210808466</v>
       </c>
     </row>
     <row r="31">
@@ -1201,37 +1201,37 @@
         <v>53</v>
       </c>
       <c r="B31">
-        <v>0.78618496410112748</v>
+        <v>0.83427428152345362</v>
       </c>
       <c r="C31">
-        <v>0.21381503589887257</v>
+        <v>0.1657257184765463</v>
       </c>
       <c r="H31">
         <v>53</v>
       </c>
       <c r="I31">
-        <v>0.20356501765990584</v>
+        <v>0.35138568421424909</v>
       </c>
       <c r="J31">
-        <v>0.79643498234009413</v>
+        <v>0.64861431578575079</v>
       </c>
       <c r="N31">
         <v>53</v>
       </c>
       <c r="O31">
-        <v>0.4886620827819475</v>
+        <v>0.34975454678925116</v>
       </c>
       <c r="P31">
-        <v>0.51133791721805255</v>
+        <v>0.65024545321074889</v>
       </c>
       <c r="T31">
         <v>53</v>
       </c>
       <c r="U31">
-        <v>0.91149009355670652</v>
+        <v>0.83827096342779417</v>
       </c>
       <c r="V31">
-        <v>0.088509906443293568</v>
+        <v>0.16172903657220586</v>
       </c>
     </row>
     <row r="32">
@@ -1239,37 +1239,37 @@
         <v>54</v>
       </c>
       <c r="B32">
-        <v>0.78605465367468785</v>
+        <v>0.85508315976754945</v>
       </c>
       <c r="C32">
-        <v>0.21394534632531212</v>
+        <v>0.14491684023245055</v>
       </c>
       <c r="H32">
         <v>54</v>
       </c>
       <c r="I32">
-        <v>0.22892594877691635</v>
+        <v>0.38217576417730792</v>
       </c>
       <c r="J32">
-        <v>0.77107405122308359</v>
+        <v>0.61782423582269219</v>
       </c>
       <c r="N32">
         <v>54</v>
       </c>
       <c r="O32">
-        <v>0.46367591176226031</v>
+        <v>0.33972017929233211</v>
       </c>
       <c r="P32">
-        <v>0.5363240882377398</v>
+        <v>0.66027982070766789</v>
       </c>
       <c r="T32">
         <v>54</v>
       </c>
       <c r="U32">
-        <v>0.89443729873961919</v>
+        <v>0.8256039953446126</v>
       </c>
       <c r="V32">
-        <v>0.10556270126038084</v>
+        <v>0.17439600465538735</v>
       </c>
     </row>
     <row r="33">
@@ -1277,37 +1277,37 @@
         <v>55</v>
       </c>
       <c r="B33">
-        <v>0.7632304290751144</v>
+        <v>0.81828597000201775</v>
       </c>
       <c r="C33">
-        <v>0.23676957092488554</v>
+        <v>0.18171402999798225</v>
       </c>
       <c r="H33">
         <v>55</v>
       </c>
       <c r="I33">
-        <v>0.2502345624660432</v>
+        <v>0.35767978658046462</v>
       </c>
       <c r="J33">
-        <v>0.74976543753395686</v>
+        <v>0.64232021341953527</v>
       </c>
       <c r="N33">
         <v>55</v>
       </c>
       <c r="O33">
-        <v>0.49318618911466655</v>
+        <v>0.44057319202459416</v>
       </c>
       <c r="P33">
-        <v>0.5068138108853335</v>
+        <v>0.55942680797540578</v>
       </c>
       <c r="T33">
         <v>55</v>
       </c>
       <c r="U33">
-        <v>0.89161439447038215</v>
+        <v>0.83784244241436567</v>
       </c>
       <c r="V33">
-        <v>0.10838560552961782</v>
+        <v>0.1621575575856343</v>
       </c>
     </row>
     <row r="34">
@@ -1315,37 +1315,37 @@
         <v>56</v>
       </c>
       <c r="B34">
-        <v>0.77610063120355743</v>
+        <v>0.78960190241396111</v>
       </c>
       <c r="C34">
-        <v>0.22389936879644262</v>
+        <v>0.21039809758603881</v>
       </c>
       <c r="H34">
         <v>56</v>
       </c>
       <c r="I34">
-        <v>0.16751003681566828</v>
+        <v>0.36402192447954418</v>
       </c>
       <c r="J34">
-        <v>0.83248996318433177</v>
+        <v>0.63597807552045582</v>
       </c>
       <c r="N34">
         <v>56</v>
       </c>
       <c r="O34">
-        <v>0.47820004944467936</v>
+        <v>0.3369287476170536</v>
       </c>
       <c r="P34">
-        <v>0.52179995055532058</v>
+        <v>0.6630712523829464</v>
       </c>
       <c r="T34">
         <v>56</v>
       </c>
       <c r="U34">
-        <v>0.90253561873414601</v>
+        <v>0.84326755552482202</v>
       </c>
       <c r="V34">
-        <v>0.097464381265853897</v>
+        <v>0.15673244447517806</v>
       </c>
     </row>
     <row r="35">
@@ -1353,37 +1353,37 @@
         <v>57</v>
       </c>
       <c r="B35">
-        <v>0.76684754313318571</v>
+        <v>0.83023298969272974</v>
       </c>
       <c r="C35">
-        <v>0.23315245686681435</v>
+        <v>0.16976701030727026</v>
       </c>
       <c r="H35">
         <v>57</v>
       </c>
       <c r="I35">
-        <v>0.26095173951507827</v>
+        <v>0.40348103375450572</v>
       </c>
       <c r="J35">
-        <v>0.73904826048492178</v>
+        <v>0.59651896624549416</v>
       </c>
       <c r="N35">
         <v>57</v>
       </c>
       <c r="O35">
-        <v>0.48204169558193927</v>
+        <v>0.22753508601689107</v>
       </c>
       <c r="P35">
-        <v>0.51795830441806079</v>
+        <v>0.77246491398310901</v>
       </c>
       <c r="T35">
         <v>57</v>
       </c>
       <c r="U35">
-        <v>0.91668758762216696</v>
+        <v>0.87165401667319731</v>
       </c>
       <c r="V35">
-        <v>0.083312412377833073</v>
+        <v>0.12834598332680275</v>
       </c>
     </row>
     <row r="36">
@@ -1391,37 +1391,37 @@
         <v>58</v>
       </c>
       <c r="B36">
-        <v>0.75885599651273072</v>
+        <v>0.76493721895849953</v>
       </c>
       <c r="C36">
-        <v>0.2411440034872693</v>
+        <v>0.23506278104150038</v>
       </c>
       <c r="H36">
         <v>58</v>
       </c>
       <c r="I36">
-        <v>0.14858348864887275</v>
+        <v>0.27109888150775857</v>
       </c>
       <c r="J36">
-        <v>0.85141651135112728</v>
+        <v>0.72890111849224137</v>
       </c>
       <c r="N36">
         <v>58</v>
       </c>
       <c r="O36">
-        <v>0.42795249743072045</v>
+        <v>0.46087932702203005</v>
       </c>
       <c r="P36">
-        <v>0.57204750256927961</v>
+        <v>0.53912067297797006</v>
       </c>
       <c r="T36">
         <v>58</v>
       </c>
       <c r="U36">
-        <v>0.91160663071099923</v>
+        <v>0.85413073764582981</v>
       </c>
       <c r="V36">
-        <v>0.088393369289000781</v>
+        <v>0.14586926235417025</v>
       </c>
     </row>
     <row r="37">
@@ -1429,37 +1429,37 @@
         <v>59</v>
       </c>
       <c r="B37">
-        <v>0.76174888354929404</v>
+        <v>0.74688051231919805</v>
       </c>
       <c r="C37">
-        <v>0.23825111645070601</v>
+        <v>0.25311948768080195</v>
       </c>
       <c r="H37">
         <v>59</v>
       </c>
       <c r="I37">
-        <v>0.21856628138109599</v>
+        <v>0.359014028060748</v>
       </c>
       <c r="J37">
-        <v>0.78143371861890398</v>
+        <v>0.640985971939252</v>
       </c>
       <c r="N37">
         <v>59</v>
       </c>
       <c r="O37">
-        <v>0.42991810973486827</v>
+        <v>0.28007792556414723</v>
       </c>
       <c r="P37">
-        <v>0.57008189026513179</v>
+        <v>0.71992207443585265</v>
       </c>
       <c r="T37">
         <v>59</v>
       </c>
       <c r="U37">
-        <v>0.89521285634674996</v>
+        <v>0.83363664770017853</v>
       </c>
       <c r="V37">
-        <v>0.10478714365325011</v>
+        <v>0.16636335229982144</v>
       </c>
     </row>
     <row r="38">
@@ -1467,37 +1467,37 @@
         <v>60</v>
       </c>
       <c r="B38">
-        <v>0.75486396300872627</v>
+        <v>0.74240450910496081</v>
       </c>
       <c r="C38">
-        <v>0.24513603699127368</v>
+        <v>0.25759549089503914</v>
       </c>
       <c r="H38">
         <v>60</v>
       </c>
       <c r="I38">
-        <v>0.21873572666748314</v>
+        <v>0.32686120829566223</v>
       </c>
       <c r="J38">
-        <v>0.7812642733325168</v>
+        <v>0.67313879170433777</v>
       </c>
       <c r="N38">
         <v>60</v>
       </c>
       <c r="O38">
-        <v>0.46467480992537158</v>
+        <v>0.28285243899481788</v>
       </c>
       <c r="P38">
-        <v>0.53532519007462842</v>
+        <v>0.71714756100518218</v>
       </c>
       <c r="T38">
         <v>60</v>
       </c>
       <c r="U38">
-        <v>0.91219426930809255</v>
+        <v>0.83962956063850014</v>
       </c>
       <c r="V38">
-        <v>0.087805730691907474</v>
+        <v>0.16037043936149981</v>
       </c>
     </row>
     <row r="39">
@@ -1505,37 +1505,37 @@
         <v>61</v>
       </c>
       <c r="B39">
-        <v>0.75294681204131209</v>
+        <v>0.80989672641314125</v>
       </c>
       <c r="C39">
-        <v>0.24705318795868783</v>
+        <v>0.1901032735868588</v>
       </c>
       <c r="H39">
         <v>61</v>
       </c>
       <c r="I39">
-        <v>0.18390635170345601</v>
+        <v>0.39928527092049754</v>
       </c>
       <c r="J39">
-        <v>0.81609364829654396</v>
+        <v>0.60071472907950252</v>
       </c>
       <c r="N39">
         <v>61</v>
       </c>
       <c r="O39">
-        <v>0.51290313351503114</v>
+        <v>0.33864741232753787</v>
       </c>
       <c r="P39">
-        <v>0.4870968664849688</v>
+        <v>0.66135258767246219</v>
       </c>
       <c r="T39">
         <v>61</v>
       </c>
       <c r="U39">
-        <v>0.8968556867477202</v>
+        <v>0.84684835460038865</v>
       </c>
       <c r="V39">
-        <v>0.10314431325227973</v>
+        <v>0.15315164539961126</v>
       </c>
     </row>
     <row r="40">
@@ -1543,37 +1543,37 @@
         <v>62</v>
       </c>
       <c r="B40">
-        <v>0.77474746074695666</v>
+        <v>0.68868225935659544</v>
       </c>
       <c r="C40">
-        <v>0.22525253925304339</v>
+        <v>0.31131774064340456</v>
       </c>
       <c r="H40">
         <v>62</v>
       </c>
       <c r="I40">
-        <v>0.1814520611084397</v>
+        <v>0.43125629940371035</v>
       </c>
       <c r="J40">
-        <v>0.81854793889156041</v>
+        <v>0.56874370059628965</v>
       </c>
       <c r="N40">
         <v>62</v>
       </c>
       <c r="O40">
-        <v>0.47145144411517514</v>
+        <v>0.086140320850890267</v>
       </c>
       <c r="P40">
-        <v>0.52854855588482497</v>
+        <v>0.91385967914910982</v>
       </c>
       <c r="T40">
         <v>62</v>
       </c>
       <c r="U40">
-        <v>0.92138275900903122</v>
+        <v>0.86985243015417557</v>
       </c>
       <c r="V40">
-        <v>0.078617240990968756</v>
+        <v>0.1301475698458244</v>
       </c>
     </row>
     <row r="41">
@@ -1581,37 +1581,37 @@
         <v>63</v>
       </c>
       <c r="B41">
-        <v>0.77197829470060531</v>
+        <v>0.73068036351890586</v>
       </c>
       <c r="C41">
-        <v>0.22802170529939467</v>
+        <v>0.26931963648109408</v>
       </c>
       <c r="H41">
         <v>63</v>
       </c>
       <c r="I41">
-        <v>0.14862952941720711</v>
+        <v>0.33739767247571678</v>
       </c>
       <c r="J41">
-        <v>0.85137047058279303</v>
+        <v>0.66260232752428316</v>
       </c>
       <c r="N41">
         <v>63</v>
       </c>
       <c r="O41">
-        <v>0.41841039446198558</v>
+        <v>0.072554513742908874</v>
       </c>
       <c r="P41">
-        <v>0.58158960553801453</v>
+        <v>0.92744548625709111</v>
       </c>
       <c r="T41">
         <v>63</v>
       </c>
       <c r="U41">
-        <v>0.9171792465723142</v>
+        <v>0.87939378231651721</v>
       </c>
       <c r="V41">
-        <v>0.082820753427685787</v>
+        <v>0.12060621768348283</v>
       </c>
     </row>
     <row r="42">
@@ -1619,37 +1619,37 @@
         <v>64</v>
       </c>
       <c r="B42">
-        <v>0.72228199973601126</v>
+        <v>0.63992820014109308</v>
       </c>
       <c r="C42">
-        <v>0.27771800026398868</v>
+        <v>0.36007179985890686</v>
       </c>
       <c r="H42">
         <v>64</v>
       </c>
       <c r="I42">
-        <v>0.20663868059157756</v>
+        <v>0.39509586365203347</v>
       </c>
       <c r="J42">
-        <v>0.79336131940842258</v>
+        <v>0.60490413634796658</v>
       </c>
       <c r="N42">
         <v>64</v>
       </c>
       <c r="O42">
-        <v>0.47980165743832348</v>
+        <v>0.4491602597516951</v>
       </c>
       <c r="P42">
-        <v>0.52019834256167663</v>
+        <v>0.55083974024830495</v>
       </c>
       <c r="T42">
         <v>64</v>
       </c>
       <c r="U42">
-        <v>0.91843677877128604</v>
+        <v>0.87128452193687045</v>
       </c>
       <c r="V42">
-        <v>0.081563221228713914</v>
+        <v>0.1287154780631295</v>
       </c>
     </row>
     <row r="43">
@@ -1657,37 +1657,37 @@
         <v>65</v>
       </c>
       <c r="B43">
-        <v>0.73010760972375965</v>
+        <v>0.62679094980454209</v>
       </c>
       <c r="C43">
-        <v>0.26989239027624035</v>
+        <v>0.37320905019545786</v>
       </c>
       <c r="H43">
         <v>65</v>
       </c>
       <c r="I43">
-        <v>0.13844965185061459</v>
+        <v>0.32162990222717919</v>
       </c>
       <c r="J43">
-        <v>0.86155034814938547</v>
+        <v>0.67837009777282087</v>
       </c>
       <c r="N43">
         <v>65</v>
       </c>
       <c r="O43">
-        <v>0.4575957106870937</v>
+        <v>0</v>
       </c>
       <c r="P43">
-        <v>0.54240428931290641</v>
+        <v>1</v>
       </c>
       <c r="T43">
         <v>65</v>
       </c>
       <c r="U43">
-        <v>0.91730965099728101</v>
+        <v>0.90777023941198554</v>
       </c>
       <c r="V43">
-        <v>0.08269034900271903</v>
+        <v>0.092229760588014548</v>
       </c>
     </row>
     <row r="44">
@@ -1695,37 +1695,37 @@
         <v>66</v>
       </c>
       <c r="B44">
-        <v>0.77154093284825898</v>
+        <v>0.73726298338906981</v>
       </c>
       <c r="C44">
-        <v>0.228459067151741</v>
+        <v>0.26273701661093024</v>
       </c>
       <c r="H44">
         <v>66</v>
       </c>
       <c r="I44">
-        <v>0.2047695498746557</v>
+        <v>0.095929724944601946</v>
       </c>
       <c r="J44">
-        <v>0.79523045012534432</v>
+        <v>0.90407027505539805</v>
       </c>
       <c r="N44">
         <v>66</v>
       </c>
       <c r="O44">
-        <v>0.49228679328737662</v>
+        <v>0.12635493674229509</v>
       </c>
       <c r="P44">
-        <v>0.50771320671262332</v>
+        <v>0.87364506325770486</v>
       </c>
       <c r="T44">
         <v>66</v>
       </c>
       <c r="U44">
-        <v>0.91942533081860867</v>
+        <v>0.89643088551181838</v>
       </c>
       <c r="V44">
-        <v>0.080574669181391403</v>
+        <v>0.10356911448818173</v>
       </c>
     </row>
     <row r="45">
@@ -1733,37 +1733,37 @@
         <v>67</v>
       </c>
       <c r="B45">
-        <v>0.74017266413484661</v>
+        <v>1</v>
       </c>
       <c r="C45">
-        <v>0.25982733586515339</v>
+        <v>0</v>
       </c>
       <c r="H45">
         <v>67</v>
       </c>
       <c r="I45">
-        <v>0.16753186512596704</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>0.83246813487403293</v>
+        <v>1</v>
       </c>
       <c r="N45">
         <v>67</v>
       </c>
       <c r="O45">
-        <v>0.52477069932493337</v>
+        <v>0.4500422748680698</v>
       </c>
       <c r="P45">
-        <v>0.47522930067506663</v>
+        <v>0.54995772513193031</v>
       </c>
       <c r="T45">
         <v>67</v>
       </c>
       <c r="U45">
-        <v>0.9132343861928961</v>
+        <v>0.87560340241037027</v>
       </c>
       <c r="V45">
-        <v>0.086765613807103834</v>
+        <v>0.12439659758962972</v>
       </c>
     </row>
     <row r="46">
@@ -1771,37 +1771,37 @@
         <v>68</v>
       </c>
       <c r="B46">
-        <v>0.70719066428807098</v>
+        <v>0.63830825368440691</v>
       </c>
       <c r="C46">
-        <v>0.29280933571192902</v>
+        <v>0.36169174631559325</v>
       </c>
       <c r="H46">
         <v>68</v>
       </c>
       <c r="I46">
-        <v>0.16009840303254144</v>
+        <v>0.31819306763331473</v>
       </c>
       <c r="J46">
-        <v>0.8399015969674587</v>
+        <v>0.68180693236668521</v>
       </c>
       <c r="N46">
         <v>68</v>
       </c>
       <c r="O46">
-        <v>0.45318572527273732</v>
+        <v>1</v>
       </c>
       <c r="P46">
-        <v>0.54681427472726263</v>
+        <v>0</v>
       </c>
       <c r="T46">
         <v>68</v>
       </c>
       <c r="U46">
-        <v>0.92162893526330347</v>
+        <v>0.89441511945677277</v>
       </c>
       <c r="V46">
-        <v>0.078371064736696514</v>
+        <v>0.10558488054322732</v>
       </c>
     </row>
     <row r="47">
@@ -1809,37 +1809,37 @@
         <v>69</v>
       </c>
       <c r="B47">
-        <v>0.7441588618511803</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <v>0.25584113814881976</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <v>69</v>
       </c>
       <c r="I47">
-        <v>0.25541255267519963</v>
+        <v>0.41368908303686458</v>
       </c>
       <c r="J47">
-        <v>0.74458744732480042</v>
+        <v>0.58631091696313542</v>
       </c>
       <c r="N47">
         <v>69</v>
       </c>
       <c r="O47">
-        <v>0.45265201406039934</v>
+        <v>0.53570623249568872</v>
       </c>
       <c r="P47">
-        <v>0.54734798593960066</v>
+        <v>0.46429376750431123</v>
       </c>
       <c r="T47">
         <v>69</v>
       </c>
       <c r="U47">
-        <v>0.89452397879033241</v>
+        <v>0.78879595979527806</v>
       </c>
       <c r="V47">
-        <v>0.10547602120966754</v>
+        <v>0.21120404020472192</v>
       </c>
     </row>
     <row r="48">
@@ -1847,37 +1847,37 @@
         <v>70</v>
       </c>
       <c r="B48">
-        <v>0.71383889355129471</v>
+        <v>0.41263645897054474</v>
       </c>
       <c r="C48">
-        <v>0.28616110644870535</v>
+        <v>0.58736354102945521</v>
       </c>
       <c r="H48">
         <v>70</v>
       </c>
       <c r="I48">
-        <v>0.18134275527907742</v>
+        <v>0.19635461386120126</v>
       </c>
       <c r="J48">
-        <v>0.81865724472092249</v>
+        <v>0.80364538613879866</v>
       </c>
       <c r="N48">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O48">
-        <v>0.46862478819247694</v>
+        <v>0</v>
       </c>
       <c r="P48">
-        <v>0.53137521180752312</v>
+        <v>1</v>
       </c>
       <c r="T48">
         <v>70</v>
       </c>
       <c r="U48">
-        <v>0.90162690756671937</v>
+        <v>0.76008264487794341</v>
       </c>
       <c r="V48">
-        <v>0.098373092433280712</v>
+        <v>0.23991735512205661</v>
       </c>
     </row>
     <row r="49">
@@ -1885,37 +1885,37 @@
         <v>71</v>
       </c>
       <c r="B49">
-        <v>0.72375499434769275</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>0.2762450056523072</v>
+        <v>0</v>
       </c>
       <c r="H49">
         <v>71</v>
       </c>
       <c r="I49">
-        <v>0.25426089767256049</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>0.74573910232743956</v>
+        <v>1</v>
       </c>
       <c r="N49">
         <v>71</v>
       </c>
       <c r="O49">
-        <v>0.4900185667605238</v>
+        <v>0.6408464943164327</v>
       </c>
       <c r="P49">
-        <v>0.50998143323947609</v>
+        <v>0.35915350568356735</v>
       </c>
       <c r="T49">
         <v>71</v>
       </c>
       <c r="U49">
-        <v>0.89866214184891891</v>
+        <v>0.77949351140032541</v>
       </c>
       <c r="V49">
-        <v>0.10133785815108108</v>
+        <v>0.2205064885996745</v>
       </c>
     </row>
     <row r="50">
@@ -1950,10 +1950,10 @@
         <v>72</v>
       </c>
       <c r="U50">
-        <v>0.88814926712517495</v>
+        <v>0.74395657504095647</v>
       </c>
       <c r="V50">
-        <v>0.11185073287482498</v>
+        <v>0.25604342495904359</v>
       </c>
     </row>
     <row r="51">
@@ -1988,10 +1988,10 @@
         <v>73</v>
       </c>
       <c r="U51">
-        <v>0.8961663544328663</v>
+        <v>1</v>
       </c>
       <c r="V51">
-        <v>0.10383364556713365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2026,10 +2026,10 @@
         <v>74</v>
       </c>
       <c r="U52">
-        <v>0.9153095652643336</v>
+        <v>1</v>
       </c>
       <c r="V52">
-        <v>0.084690434735666481</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2064,10 +2064,10 @@
         <v>75</v>
       </c>
       <c r="U53">
-        <v>0.8752254383437017</v>
+        <v>1</v>
       </c>
       <c r="V53">
-        <v>0.12477456165629827</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>